<commit_message>
Finalised ISr function and began testthat ISR script.  Updated documentation.
</commit_message>
<xml_diff>
--- a/tests/testthat/APHO Tool for common PH Stats and CIs_adapted.xlsx
+++ b/tests/testthat/APHO Tool for common PH Stats and CIs_adapted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11175" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11175" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="5" r:id="rId1"/>
@@ -4487,7 +4487,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="13">
+  <numFmts count="14">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
@@ -4501,6 +4501,7 @@
     <numFmt numFmtId="174" formatCode="??0.00000"/>
     <numFmt numFmtId="175" formatCode="???,??0"/>
     <numFmt numFmtId="176" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="177" formatCode="0.00000"/>
   </numFmts>
   <fonts count="69" x14ac:knownFonts="1">
     <font>
@@ -5671,7 +5672,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6152,6 +6153,12 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="27" fillId="24" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="27" fillId="24" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -10358,7 +10365,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q122"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10492,12 +10501,12 @@
         <v>65000</v>
       </c>
       <c r="E6" s="93">
-        <f>IF(B6=0,0,IF(B6&lt;389,CHIINV(0.5+$E$10/200,2*B6)/2,B6*(1-1/(9*B6)-NORMSINV(0.5+$E$10/200)/3/SQRT(B6))^3))/C6*$F$10</f>
-        <v>50165.627729234264</v>
+        <f>IF(B6=0,0,IF(B6&lt;10,CHIINV(0.5+$E$10/200,2*B6)/2,B6*(1-1/(9*B6)-NORMSINV(0.5+$E$10/200)/3/SQRT(B6))^3))/C6*$F$10</f>
+        <v>50163.187710459453</v>
       </c>
       <c r="F6" s="94">
-        <f>IF(B6&lt;389,CHIINV(0.5-$E$10/200,2*B6+2)/2,(B6+1)*(1-1/(9*(B6+1))+NORMSINV(0.5+$E$10/200)/3/SQRT(B6+1))^3)/C6*$F$10</f>
-        <v>82847.835815871571</v>
+        <f>IF(B6&lt;10,CHIINV(0.5-$E$10/200,2*B6+2)/2,(B6+1)*(1-1/(9*(B6+1))+NORMSINV(0.5+$E$10/200)/3/SQRT(B6+1))^3)/C6*$F$10</f>
+        <v>82849.138545939844</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -11934,7 +11943,6 @@
       <c r="P122" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="E4:F4"/>
   </mergeCells>
@@ -13737,7 +13745,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:Q167"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13893,7 +13903,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="70">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="D7" s="78">
         <v>636</v>
@@ -13925,7 +13935,7 @@
         <v>63</v>
       </c>
       <c r="C8" s="71">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D8" s="79">
         <v>558</v>
@@ -13957,7 +13967,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="71">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D9" s="79">
         <v>609</v>
@@ -13989,7 +13999,7 @@
         <v>65</v>
       </c>
       <c r="C10" s="72">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D10" s="80">
         <v>543</v>
@@ -14021,7 +14031,7 @@
         <v>71</v>
       </c>
       <c r="C11" s="72">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D11" s="80">
         <v>384</v>
@@ -14053,7 +14063,7 @@
         <v>72</v>
       </c>
       <c r="C12" s="72">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D12" s="80">
         <v>594</v>
@@ -14085,7 +14095,7 @@
         <v>73</v>
       </c>
       <c r="C13" s="72">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D13" s="80">
         <v>669</v>
@@ -14117,7 +14127,7 @@
         <v>74</v>
       </c>
       <c r="C14" s="72">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D14" s="80">
         <v>843</v>
@@ -14149,7 +14159,7 @@
         <v>75</v>
       </c>
       <c r="C15" s="72">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D15" s="80">
         <v>660</v>
@@ -14181,7 +14191,7 @@
         <v>76</v>
       </c>
       <c r="C16" s="72">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="D16" s="80">
         <v>576</v>
@@ -14213,7 +14223,7 @@
         <v>70</v>
       </c>
       <c r="C17" s="72">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D17" s="80">
         <v>606</v>
@@ -14245,7 +14255,7 @@
         <v>69</v>
       </c>
       <c r="C18" s="72">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="D18" s="80">
         <v>522</v>
@@ -14277,7 +14287,7 @@
         <v>68</v>
       </c>
       <c r="C19" s="72">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D19" s="80">
         <v>426</v>
@@ -14309,7 +14319,7 @@
         <v>67</v>
       </c>
       <c r="C20" s="72">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="D20" s="80">
         <v>273</v>
@@ -14341,7 +14351,7 @@
         <v>66</v>
       </c>
       <c r="C21" s="72">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D21" s="80">
         <v>300</v>
@@ -14373,7 +14383,7 @@
         <v>81</v>
       </c>
       <c r="C22" s="73">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D22" s="81">
         <v>288</v>
@@ -14405,7 +14415,7 @@
         <v>82</v>
       </c>
       <c r="C23" s="73">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="D23" s="81">
         <v>153</v>
@@ -14437,7 +14447,7 @@
         <v>297</v>
       </c>
       <c r="C24" s="73">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="D24" s="81">
         <v>123</v>
@@ -14469,7 +14479,7 @@
         <v>296</v>
       </c>
       <c r="C25" s="73">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="D25" s="81">
         <v>207</v>
@@ -14502,7 +14512,7 @@
       </c>
       <c r="C26" s="108">
         <f>SUM(C7:C25)</f>
-        <v>895</v>
+        <v>91</v>
       </c>
       <c r="D26" s="109">
         <f>SUM(D7:D25)</f>
@@ -14589,7 +14599,7 @@
       </c>
       <c r="E30" s="154" t="str">
         <f>TEXT($E$36,"General")&amp;"% Confidence Interval"</f>
-        <v>95% Confidence Interval</v>
+        <v>99.8% Confidence Interval</v>
       </c>
       <c r="F30" s="156"/>
       <c r="G30" s="24"/>
@@ -14632,23 +14642,23 @@
     <row r="32" spans="2:15" s="26" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="82">
         <f>$C$26</f>
-        <v>895</v>
+        <v>91</v>
       </c>
       <c r="C32" s="89">
         <f>$H$26</f>
         <v>868.50151748646806</v>
       </c>
-      <c r="D32" s="93">
+      <c r="D32" s="159">
         <f>IF(B32&lt;0,"#NUM!",B32/C32*$F$36)</f>
-        <v>103.0510577103217</v>
-      </c>
-      <c r="E32" s="93">
-        <f>IF(B32=0,0,IF(B32&lt;389,CHIINV(0.5+$E$36/200,2*B32)/2,B32*(1-1/(9*B32)-NORMSINV(0.5+$E$36/200)/3/SQRT(B32))^3))/C32*$F$36</f>
-        <v>96.409377931556691</v>
-      </c>
-      <c r="F32" s="94">
-        <f>IF(B32&lt;389,CHIINV(0.5-$E$36/200,2*B32+2)/2,(B32+1)*(1-1/(9*(B32+1))+NORMSINV(0.5+$E$36/200)/3/SQRT(B32+1))^3)/C32*$F$36</f>
-        <v>110.02973422891613</v>
+        <v>10.477817040937738</v>
+      </c>
+      <c r="E32" s="159">
+        <f>IF(B32=0,0,IF(B32&lt;10,CHIINV(0.5+$E$36/200,2*B32)/2,B32*(1-1/(9*B32)-NORMSINV(0.5+$E$36/200)/3/SQRT(B32))^3))/C32*$F$36</f>
+        <v>7.4064115794269885</v>
+      </c>
+      <c r="F32" s="160">
+        <f>IF(B32&lt;10,CHIINV(0.5-$E$36/200,2*B32+2)/2,(B32+1)*(1-1/(9*(B32+1))+NORMSINV(0.5+$E$36/200)/3/SQRT(B32+1))^3)/C32*$F$36</f>
+        <v>14.338405403444703</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
@@ -14684,7 +14694,7 @@
     <row r="36" spans="2:16" s="25" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D36" s="46"/>
       <c r="E36" s="32">
-        <v>95</v>
+        <v>99.8</v>
       </c>
       <c r="F36" s="92">
         <v>100</v>
@@ -14694,7 +14704,7 @@
       </c>
       <c r="H36" s="127">
         <f>1-E36/100</f>
-        <v>5.0000000000000044E-2</v>
+        <v>2.0000000000000018E-3</v>
       </c>
     </row>
     <row r="37" spans="2:16" s="26" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14743,7 +14753,7 @@
       </c>
       <c r="E39" s="154" t="str">
         <f>TEXT($E$36,"General")&amp;"% Confidence Interval"</f>
-        <v>95% Confidence Interval</v>
+        <v>99.8% Confidence Interval</v>
       </c>
       <c r="F39" s="156"/>
       <c r="G39" s="24"/>
@@ -14785,7 +14795,7 @@
     <row r="41" spans="2:16" s="26" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="82">
         <f>$C$26</f>
-        <v>895</v>
+        <v>91</v>
       </c>
       <c r="C41" s="89">
         <f>$H$26</f>
@@ -14793,15 +14803,15 @@
       </c>
       <c r="D41" s="95">
         <f>IF(B41&lt;0,"#NUM!",B41/C41*$D$45)</f>
-        <v>10014.578176786832</v>
+        <v>1018.2420269135216</v>
       </c>
       <c r="E41" s="95">
-        <f>IF(B41=0,0,IF(B41&lt;389,CHIINV(0.5+$E$45/200,2*B41)/2,B41*(1-1/(9*B41)-NORMSINV(0.5+$E$45/200)/3/SQRT(B41))^3))/C41*$D$45</f>
-        <v>9369.1348126187768</v>
+        <f>IF(B41=0,0,IF(B41&lt;10,CHIINV(0.5+$E$45/200,2*B41)/2,B41*(1-1/(9*B41)-NORMSINV(0.5+$E$45/200)/3/SQRT(B41))^3))/C41*$D$45</f>
+        <v>819.80264950202934</v>
       </c>
       <c r="F41" s="96">
-        <f>IF(B41&lt;389,CHIINV(0.5-$E$45/200,2*B41+2)/2,(B41+1)*(1-1/(9*(B41+1))+NORMSINV(0.5+$E$45/200)/3/SQRT(B41+1))^3)/C41*$D$45</f>
-        <v>10692.771133936561</v>
+        <f>IF(B41&lt;10,CHIINV(0.5-$E$45/200,2*B41+2)/2,(B41+1)*(1-1/(9*(B41+1))+NORMSINV(0.5+$E$45/200)/3/SQRT(B41+1))^3)/C41*$D$45</f>
+        <v>1250.1887682774923</v>
       </c>
       <c r="G41" s="24"/>
       <c r="H41" s="24"/>
@@ -15602,7 +15612,7 @@
       </c>
       <c r="H89" s="123">
         <f>H92/H93</f>
-        <v>1.030510577103217</v>
+        <v>0.10477817040937738</v>
       </c>
     </row>
     <row r="90" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15624,7 +15634,7 @@
       </c>
       <c r="H92" s="127">
         <f>SUM(C7:C25)</f>
-        <v>895</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.2">
@@ -15736,7 +15746,7 @@
       </c>
       <c r="H106" s="123">
         <f>H118/H93</f>
-        <v>0.96409377931556683</v>
+        <v>7.4064115794269872E-2</v>
       </c>
       <c r="J106" s="2"/>
       <c r="K106" s="10"/>
@@ -15765,7 +15775,7 @@
       </c>
       <c r="H109" s="123">
         <f>H121/H93</f>
-        <v>1.1002973422891613</v>
+        <v>0.14338405403444704</v>
       </c>
       <c r="J109" s="2"/>
       <c r="K109" s="10"/>
@@ -15850,7 +15860,7 @@
       </c>
       <c r="H118" s="123">
         <f>H92*(1-1/(9*H92)-H124/(3*SQRT(H92)))^3</f>
-        <v>837.31691033483389</v>
+        <v>64.324796958616872</v>
       </c>
       <c r="J118" s="2"/>
       <c r="K118" s="10"/>
@@ -15878,7 +15888,7 @@
       </c>
       <c r="H121" s="123">
         <f>(H92+1)*(1-1/(9*(H92+1))+H124/(3*SQRT(H92+1)))^3</f>
-        <v>955.60991146446429</v>
+        <v>124.52926851227897</v>
       </c>
       <c r="J121" s="2"/>
       <c r="K121" s="10"/>
@@ -15908,7 +15918,7 @@
       </c>
       <c r="H124" s="123">
         <f>NORMSINV(1-H36/2)</f>
-        <v>1.9599639845400536</v>
+        <v>3.0902323061678132</v>
       </c>
       <c r="J124" s="2"/>
       <c r="K124" s="10"/>
@@ -15998,7 +16008,7 @@
       </c>
       <c r="H136" s="123">
         <f>H141/2</f>
-        <v>837.31746186084513</v>
+        <v>64.343294242181898</v>
       </c>
       <c r="J136" s="2"/>
       <c r="K136" s="10"/>
@@ -16030,7 +16040,7 @@
       </c>
       <c r="H139" s="123">
         <f>H143/2</f>
-        <v>955.60944311267701</v>
+        <v>124.50901956736195</v>
       </c>
       <c r="J139" s="2"/>
       <c r="K139" s="10"/>
@@ -16057,7 +16067,7 @@
       </c>
       <c r="H141" s="123">
         <f>CHIINV(1-H36/2,2*H92)</f>
-        <v>1674.6349237216903</v>
+        <v>128.6865884843638</v>
       </c>
       <c r="J141" s="2"/>
       <c r="K141" s="10"/>
@@ -16081,7 +16091,7 @@
       </c>
       <c r="H143" s="123">
         <f>CHIINV(H36/2,2*H92+2)</f>
-        <v>1911.218886225354</v>
+        <v>249.01803913472389</v>
       </c>
       <c r="J143" s="2"/>
       <c r="K143" s="10"/>
@@ -16442,7 +16452,6 @@
       <c r="P167" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E39:F39"/>
@@ -16588,8 +16597,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>